<commit_message>
Working on the communication approach part
</commit_message>
<xml_diff>
--- a/Demonstation/Communication/ExxonMobil_analysis.xlsx
+++ b/Demonstation/Communication/ExxonMobil_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ludov\Desktop\Thesis\Research itself\Step 3 - Design Development\1. Communication\Validating\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ludov\Desktop\Thesis\Chapters\GitHub repository\Demonstation\Communication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8405FCBC-103F-4C01-ADEE-27EE927AAB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C7A028-5AD0-4D83-B029-B6C5800BC28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -1417,10 +1417,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1431,9 +1434,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1771,7 +1771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1886,7 +1886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74647B76-71EF-42A2-9AC4-7BB4F232E6B9}">
   <dimension ref="A1:G174"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1958,13 +1958,13 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="27" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="15" t="s">
@@ -1978,9 +1978,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="15" t="s">
         <v>41</v>
       </c>
@@ -1989,9 +1989,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="15" t="s">
         <v>42</v>
       </c>
@@ -2000,9 +2000,9 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="15" t="s">
         <v>44</v>
       </c>
@@ -2011,9 +2011,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="15" t="s">
         <v>45</v>
       </c>
@@ -2022,9 +2022,9 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="15" t="s">
         <v>51</v>
       </c>
@@ -2033,9 +2033,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="15" t="s">
         <v>46</v>
       </c>
@@ -2044,9 +2044,9 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="15" t="s">
         <v>52</v>
       </c>
@@ -2055,9 +2055,9 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="15" t="s">
         <v>47</v>
       </c>
@@ -2066,9 +2066,9 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="15" t="s">
         <v>48</v>
       </c>
@@ -2077,9 +2077,9 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="15" t="s">
         <v>53</v>
       </c>
@@ -2088,9 +2088,9 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="15" t="s">
         <v>49</v>
       </c>
@@ -2099,9 +2099,9 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="15" t="s">
         <v>50</v>
       </c>
@@ -2110,9 +2110,9 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="15" t="s">
         <v>54</v>
       </c>
@@ -2121,9 +2121,9 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="15" t="s">
         <v>55</v>
       </c>
@@ -2132,9 +2132,9 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="15" t="s">
         <v>56</v>
       </c>
@@ -2143,9 +2143,9 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="15" t="s">
         <v>57</v>
       </c>
@@ -2154,9 +2154,9 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="15" t="s">
         <v>58</v>
       </c>
@@ -2165,9 +2165,9 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="15" t="s">
         <v>59</v>
       </c>
@@ -2176,9 +2176,9 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="15" t="s">
         <v>60</v>
       </c>
@@ -2187,9 +2187,9 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="15" t="s">
         <v>61</v>
       </c>
@@ -2198,9 +2198,9 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="15" t="s">
         <v>62</v>
       </c>
@@ -2209,9 +2209,9 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="15" t="s">
         <v>63</v>
       </c>
@@ -2220,9 +2220,9 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="15" t="s">
         <v>64</v>
       </c>
@@ -2231,9 +2231,9 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
       <c r="D30" s="15" t="s">
         <v>65</v>
       </c>
@@ -2242,9 +2242,9 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
       <c r="D31" s="15" t="s">
         <v>66</v>
       </c>
@@ -2253,9 +2253,9 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
       <c r="D32" s="15" t="s">
         <v>67</v>
       </c>
@@ -2264,9 +2264,9 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
       <c r="D33" s="15" t="s">
         <v>68</v>
       </c>
@@ -2275,9 +2275,9 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="15" t="s">
         <v>69</v>
       </c>
@@ -2286,9 +2286,9 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
       <c r="D35" s="15" t="s">
         <v>70</v>
       </c>
@@ -2297,9 +2297,9 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
       <c r="D36" s="15" t="s">
         <v>71</v>
       </c>
@@ -2308,9 +2308,9 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="15" t="s">
         <v>72</v>
       </c>
@@ -2319,9 +2319,9 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
       <c r="D38" s="15" t="s">
         <v>73</v>
       </c>
@@ -2330,9 +2330,9 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
       <c r="D39" s="15" t="s">
         <v>74</v>
       </c>
@@ -2341,9 +2341,9 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
       <c r="D40" s="15" t="s">
         <v>75</v>
       </c>
@@ -2352,9 +2352,9 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="25"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
       <c r="D41" s="15" t="s">
         <v>76</v>
       </c>
@@ -2363,9 +2363,9 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
       <c r="D42" s="15" t="s">
         <v>77</v>
       </c>
@@ -2374,9 +2374,9 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
       <c r="D43" s="15" t="s">
         <v>78</v>
       </c>
@@ -2385,9 +2385,9 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
       <c r="D44" s="15" t="s">
         <v>79</v>
       </c>
@@ -2396,9 +2396,9 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="25"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
       <c r="D45" s="15" t="s">
         <v>80</v>
       </c>
@@ -2407,9 +2407,9 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="25"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
       <c r="D46" s="15" t="s">
         <v>81</v>
       </c>
@@ -3643,24 +3643,24 @@
   </sheetData>
   <autoFilter ref="D6:E146" xr:uid="{74647B76-71EF-42A2-9AC4-7BB4F232E6B9}"/>
   <mergeCells count="18">
+    <mergeCell ref="A6:A46"/>
+    <mergeCell ref="B6:B46"/>
+    <mergeCell ref="C6:C46"/>
+    <mergeCell ref="C47:C63"/>
+    <mergeCell ref="B47:B63"/>
+    <mergeCell ref="A47:A63"/>
+    <mergeCell ref="C64:C103"/>
+    <mergeCell ref="B64:B103"/>
+    <mergeCell ref="A64:A103"/>
+    <mergeCell ref="C104:C122"/>
+    <mergeCell ref="B104:B122"/>
+    <mergeCell ref="A104:A122"/>
     <mergeCell ref="C123:C129"/>
     <mergeCell ref="B123:B129"/>
     <mergeCell ref="A123:A129"/>
     <mergeCell ref="C130:C146"/>
     <mergeCell ref="B130:B146"/>
     <mergeCell ref="A130:A146"/>
-    <mergeCell ref="C64:C103"/>
-    <mergeCell ref="B64:B103"/>
-    <mergeCell ref="A64:A103"/>
-    <mergeCell ref="C104:C122"/>
-    <mergeCell ref="B104:B122"/>
-    <mergeCell ref="A104:A122"/>
-    <mergeCell ref="A6:A46"/>
-    <mergeCell ref="B6:B46"/>
-    <mergeCell ref="C6:C46"/>
-    <mergeCell ref="C47:C63"/>
-    <mergeCell ref="B47:B63"/>
-    <mergeCell ref="A47:A63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3677,15 +3677,15 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="25" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="30">
+      <c r="A2" s="25">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -3696,7 +3696,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="30">
+      <c r="A3" s="25">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -3707,7 +3707,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="30">
+      <c r="A4" s="25">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -3718,7 +3718,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="30">
+      <c r="A5" s="25">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -3729,7 +3729,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="30">
+      <c r="A6" s="25">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -3740,7 +3740,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="30">
+      <c r="A7" s="25">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -3751,7 +3751,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="30">
+      <c r="A8" s="25">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -3762,7 +3762,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="30">
+      <c r="A9" s="25">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -3773,7 +3773,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="30">
+      <c r="A10" s="25">
         <v>8</v>
       </c>
       <c r="B10" t="s">
@@ -3784,7 +3784,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="30">
+      <c r="A11" s="25">
         <v>9</v>
       </c>
       <c r="B11" t="s">
@@ -3795,7 +3795,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="30">
+      <c r="A12" s="25">
         <v>10</v>
       </c>
       <c r="B12" t="s">
@@ -3806,7 +3806,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="30">
+      <c r="A13" s="25">
         <v>11</v>
       </c>
       <c r="B13" t="s">
@@ -3817,7 +3817,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="30">
+      <c r="A14" s="25">
         <v>12</v>
       </c>
       <c r="B14" t="s">
@@ -3828,7 +3828,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="30">
+      <c r="A15" s="25">
         <v>13</v>
       </c>
       <c r="B15" t="s">
@@ -3839,7 +3839,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="30">
+      <c r="A16" s="25">
         <v>14</v>
       </c>
       <c r="B16" t="s">
@@ -3850,7 +3850,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="30">
+      <c r="A17" s="25">
         <v>15</v>
       </c>
       <c r="B17" t="s">
@@ -3861,7 +3861,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="30">
+      <c r="A18" s="25">
         <v>16</v>
       </c>
       <c r="B18" t="s">
@@ -3872,7 +3872,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="30">
+      <c r="A19" s="25">
         <v>17</v>
       </c>
       <c r="B19" t="s">
@@ -3883,7 +3883,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="30">
+      <c r="A20" s="25">
         <v>18</v>
       </c>
       <c r="B20" t="s">
@@ -3894,7 +3894,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="30">
+      <c r="A21" s="25">
         <v>19</v>
       </c>
       <c r="B21" t="s">
@@ -3905,7 +3905,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="30">
+      <c r="A22" s="25">
         <v>20</v>
       </c>
       <c r="B22" t="s">
@@ -3916,7 +3916,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="30">
+      <c r="A23" s="25">
         <v>21</v>
       </c>
       <c r="B23" t="s">
@@ -3927,7 +3927,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="30">
+      <c r="A24" s="25">
         <v>22</v>
       </c>
       <c r="B24" t="s">
@@ -3938,7 +3938,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="30">
+      <c r="A25" s="25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
@@ -3949,7 +3949,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="30">
+      <c r="A26" s="25">
         <v>24</v>
       </c>
       <c r="B26" t="s">
@@ -3960,7 +3960,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="30">
+      <c r="A27" s="25">
         <v>25</v>
       </c>
       <c r="B27" t="s">
@@ -3971,7 +3971,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="30">
+      <c r="A28" s="25">
         <v>26</v>
       </c>
       <c r="B28" t="s">
@@ -3982,7 +3982,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="30">
+      <c r="A29" s="25">
         <v>27</v>
       </c>
       <c r="B29" t="s">
@@ -3993,7 +3993,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="30">
+      <c r="A30" s="25">
         <v>28</v>
       </c>
       <c r="B30" t="s">
@@ -4004,7 +4004,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="30">
+      <c r="A31" s="25">
         <v>29</v>
       </c>
       <c r="B31" t="s">
@@ -4015,7 +4015,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="30">
+      <c r="A32" s="25">
         <v>30</v>
       </c>
       <c r="B32" t="s">
@@ -4026,7 +4026,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="30">
+      <c r="A33" s="25">
         <v>31</v>
       </c>
       <c r="B33" t="s">
@@ -4037,7 +4037,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="30">
+      <c r="A34" s="25">
         <v>32</v>
       </c>
       <c r="B34" t="s">
@@ -4048,7 +4048,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="30">
+      <c r="A35" s="25">
         <v>33</v>
       </c>
       <c r="B35" t="s">
@@ -4059,7 +4059,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="30">
+      <c r="A36" s="25">
         <v>34</v>
       </c>
       <c r="B36" t="s">
@@ -4070,7 +4070,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="30">
+      <c r="A37" s="25">
         <v>35</v>
       </c>
       <c r="B37" t="s">
@@ -4081,7 +4081,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="30">
+      <c r="A38" s="25">
         <v>36</v>
       </c>
       <c r="B38" t="s">
@@ -4092,7 +4092,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="30">
+      <c r="A39" s="25">
         <v>37</v>
       </c>
       <c r="B39" t="s">
@@ -4103,7 +4103,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="30">
+      <c r="A40" s="25">
         <v>38</v>
       </c>
       <c r="B40" t="s">
@@ -4114,7 +4114,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="30">
+      <c r="A41" s="25">
         <v>39</v>
       </c>
       <c r="B41" t="s">
@@ -4125,7 +4125,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="30">
+      <c r="A42" s="25">
         <v>40</v>
       </c>
       <c r="B42" t="s">
@@ -4136,7 +4136,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="30">
+      <c r="A43" s="25">
         <v>41</v>
       </c>
       <c r="B43" t="s">
@@ -4147,7 +4147,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="30">
+      <c r="A44" s="25">
         <v>42</v>
       </c>
       <c r="B44" t="s">
@@ -4158,7 +4158,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="30">
+      <c r="A45" s="25">
         <v>43</v>
       </c>
       <c r="B45" t="s">
@@ -4169,7 +4169,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="30">
+      <c r="A46" s="25">
         <v>44</v>
       </c>
       <c r="B46" t="s">
@@ -4180,7 +4180,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="30">
+      <c r="A47" s="25">
         <v>45</v>
       </c>
       <c r="B47" t="s">
@@ -4191,7 +4191,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="30">
+      <c r="A48" s="25">
         <v>46</v>
       </c>
       <c r="B48" t="s">
@@ -4202,7 +4202,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="30">
+      <c r="A49" s="25">
         <v>47</v>
       </c>
       <c r="B49" t="s">
@@ -4213,7 +4213,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="30">
+      <c r="A50" s="25">
         <v>48</v>
       </c>
       <c r="B50" t="s">
@@ -4224,7 +4224,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="30">
+      <c r="A51" s="25">
         <v>49</v>
       </c>
       <c r="B51" t="s">
@@ -4235,7 +4235,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="30">
+      <c r="A52" s="25">
         <v>50</v>
       </c>
       <c r="B52" t="s">
@@ -4246,7 +4246,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="30">
+      <c r="A53" s="25">
         <v>51</v>
       </c>
       <c r="B53" t="s">
@@ -4257,7 +4257,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="30">
+      <c r="A54" s="25">
         <v>52</v>
       </c>
       <c r="B54" t="s">
@@ -4268,7 +4268,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="30">
+      <c r="A55" s="25">
         <v>53</v>
       </c>
       <c r="B55" t="s">
@@ -4279,7 +4279,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="30">
+      <c r="A56" s="25">
         <v>54</v>
       </c>
       <c r="B56" t="s">
@@ -4290,7 +4290,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="30">
+      <c r="A57" s="25">
         <v>55</v>
       </c>
       <c r="B57" t="s">
@@ -4301,7 +4301,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="30">
+      <c r="A58" s="25">
         <v>56</v>
       </c>
       <c r="B58" t="s">
@@ -4312,7 +4312,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="30">
+      <c r="A59" s="25">
         <v>57</v>
       </c>
       <c r="B59" t="s">
@@ -4323,7 +4323,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="30">
+      <c r="A60" s="25">
         <v>58</v>
       </c>
       <c r="B60" t="s">
@@ -4334,7 +4334,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="30">
+      <c r="A61" s="25">
         <v>59</v>
       </c>
       <c r="B61" t="s">
@@ -4345,7 +4345,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="30">
+      <c r="A62" s="25">
         <v>60</v>
       </c>
       <c r="B62" t="s">
@@ -4356,7 +4356,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="30">
+      <c r="A63" s="25">
         <v>61</v>
       </c>
       <c r="B63" t="s">
@@ -4367,7 +4367,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="30">
+      <c r="A64" s="25">
         <v>62</v>
       </c>
       <c r="B64" t="s">
@@ -4378,7 +4378,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="30">
+      <c r="A65" s="25">
         <v>63</v>
       </c>
       <c r="B65" t="s">
@@ -4389,7 +4389,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="30">
+      <c r="A66" s="25">
         <v>64</v>
       </c>
       <c r="B66" t="s">
@@ -4400,7 +4400,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="30">
+      <c r="A67" s="25">
         <v>65</v>
       </c>
       <c r="B67" t="s">
@@ -4411,7 +4411,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="30">
+      <c r="A68" s="25">
         <v>66</v>
       </c>
       <c r="B68" t="s">
@@ -4422,7 +4422,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="30">
+      <c r="A69" s="25">
         <v>67</v>
       </c>
       <c r="B69" t="s">
@@ -4433,7 +4433,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="30">
+      <c r="A70" s="25">
         <v>68</v>
       </c>
       <c r="B70" t="s">
@@ -4444,7 +4444,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="30">
+      <c r="A71" s="25">
         <v>69</v>
       </c>
       <c r="B71" t="s">
@@ -4455,7 +4455,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="30">
+      <c r="A72" s="25">
         <v>70</v>
       </c>
       <c r="B72" t="s">
@@ -4476,8 +4476,8 @@
   <dimension ref="A1:L101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6125,7 +6125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624E649E-DA39-4B02-AA56-FF1235D460CD}">
   <dimension ref="A2:G117"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J106" sqref="J106"/>
     </sheetView>
   </sheetViews>
@@ -7667,7 +7667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E1197E-DCD7-4A88-81C0-88B35634AD2B}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -7789,7 +7789,7 @@
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -7801,7 +7801,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="27"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
@@ -7824,7 +7824,7 @@
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -7836,7 +7836,7 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="28"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="1" t="s">
         <v>17</v>
       </c>
@@ -7859,7 +7859,7 @@
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="30" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -7871,7 +7871,7 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="29"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="8" t="s">
         <v>19</v>
       </c>
@@ -7908,8 +7908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233B2BEC-9732-433C-B004-47D6BE106345}">
   <dimension ref="B1:C46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>